<commit_message>
3rd change for Reusability(Summarize functions)
</commit_message>
<xml_diff>
--- a/data/output/latest.xlsx
+++ b/data/output/latest.xlsx
@@ -434,17 +434,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Seg 1-3</t>
+          <t>count_value_1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Seg 4-6</t>
+          <t>count_value_2</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Grand Total</t>
+          <t>total_count</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change _pivot_values_to_columns to rename df column names
</commit_message>
<xml_diff>
--- a/data/output/latest.xlsx
+++ b/data/output/latest.xlsx
@@ -434,17 +434,17 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>count_value_1</t>
+          <t>Seg 1-3</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>count_value_2</t>
+          <t>Seg 4-6</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>total_count</t>
+          <t>Grand_Total</t>
         </is>
       </c>
     </row>

</xml_diff>